<commit_message>
Attempted Task 1 and commit
</commit_message>
<xml_diff>
--- a/Task 1/Country-Code.xlsx
+++ b/Task 1/Country-Code.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrutimehta/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d74a8ed63f6cad3/Documents/CC4_Data_Engineer_Test/Task 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_91FAC6F3AFFE9B6EB77FC416460202662BDCDC65" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D181F6EB-F5EB-45F1-9166-4F79E109AC12}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="6260" windowWidth="24440" windowHeight="14500" xr2:uid="{F44E485E-B9EA-7D43-9A7B-5903DA87CF9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F44E485E-B9EA-7D43-9A7B-5903DA87CF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,13 +429,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BFBC7E-A506-FD4D-9138-ADD8614C8CA3}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -442,7 +441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,7 +449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>14</v>
       </c>
@@ -458,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>30</v>
       </c>
@@ -466,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>37</v>
       </c>
@@ -474,7 +473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>94</v>
       </c>
@@ -482,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>148</v>
       </c>
@@ -490,7 +489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>162</v>
       </c>
@@ -498,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>166</v>
       </c>
@@ -506,7 +505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>184</v>
       </c>
@@ -514,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>189</v>
       </c>
@@ -522,7 +521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>191</v>
       </c>
@@ -530,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>208</v>
       </c>
@@ -538,7 +537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>214</v>
       </c>
@@ -546,7 +545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>215</v>
       </c>
@@ -554,7 +553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>216</v>
       </c>

</xml_diff>